<commit_message>
-Updated SIP budget template
</commit_message>
<xml_diff>
--- a/data/AGE-WELL SIP-A Budget Template.xlsx
+++ b/data/AGE-WELL SIP-A Budget Template.xlsx
@@ -173,9 +173,6 @@
     </r>
   </si>
   <si>
-    <t>April 1, 2019 - March 31, 2020</t>
-  </si>
-  <si>
     <r>
       <t>***To estimate in-kind contributions, use CIHR In Kind Eligibility guidelines (</t>
     </r>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>In-Kind ***</t>
+  </si>
+  <si>
+    <t>April 1, 2020 - March 31, 2021</t>
   </si>
 </sst>
 </file>
@@ -535,6 +535,16 @@
     <xf numFmtId="167" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,16 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -938,7 +938,7 @@
   <dimension ref="A1:AMK31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -957,15 +957,15 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1"/>
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
       <c r="I1"/>
       <c r="K1"/>
       <c r="L1"/>
@@ -1983,63 +1983,63 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:1024" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:1024" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:1024" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:1024" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:1024" ht="6" customHeight="1" x14ac:dyDescent="0.2">
@@ -3069,32 +3069,32 @@
     </row>
     <row r="8" spans="1:1024" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="Z8"/>
     </row>
     <row r="9" spans="1:1024" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43" t="s">
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46" t="s">
         <v>10</v>
       </c>
       <c r="Z9" s="11"/>
@@ -3116,12 +3116,12 @@
         <v>15</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="46"/>
       <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="1:1024" ht="22.5" x14ac:dyDescent="0.2">
@@ -3426,16 +3426,16 @@
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="A27" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3443,22 +3443,22 @@
     <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A27:H27"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:H3"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.27013888888888898" right="0.25" top="0.32013888888888897" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -3486,63 +3486,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:8" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:8" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" spans="1:8" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -3553,31 +3553,31 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43" t="s">
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3603,7 +3603,7 @@
       <c r="G9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="43"/>
+      <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -3876,24 +3876,19 @@
       <c r="A23" s="39"/>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:H3"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="H8:H9"/>
@@ -3903,6 +3898,11 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:H3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>